<commit_message>
use more readable named range
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/report/Travel Management.xlsx
+++ b/src/main/webapp/WEB-INF/books/report/Travel Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F66FAC-CA42-164D-919A-5FA4CC18E95D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412558CF-C821-574A-9323-BE8189EF98E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
   </sheets>
   <definedNames>
     <definedName name="Build">Sheet1!$E$11</definedName>
-    <definedName name="FormTable">Sheet1!$C$5:$D$9</definedName>
     <definedName name="Templates">Table3[Travel Form]</definedName>
+    <definedName name="TemplateTable">Sheet1!$C$5:$D$9</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -765,7 +765,7 @@
   <dimension ref="B2:Q38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
set font as Arial to display a chebox correctly
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/report/Travel Management.xlsx
+++ b/src/main/webapp/WEB-INF/books/report/Travel Management.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412558CF-C821-574A-9323-BE8189EF98E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DF9EC9-5CF0-A140-A081-2DA3E301BE6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,8 @@
     <font>
       <sz val="20"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -217,20 +216,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="20"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -250,27 +270,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -458,8 +457,8 @@
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Selection" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Travel Form" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Selection" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Travel Form" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark3 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -765,7 +764,7 @@
   <dimension ref="B2:Q38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,12 +780,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -794,10 +793,10 @@
     </row>
     <row r="3" spans="2:9" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.25">
@@ -815,8 +814,8 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="16" t="s">
+    <row r="6" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -827,8 +826,8 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="16" t="s">
+    <row r="7" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -839,8 +838,8 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="16" t="s">
+    <row r="8" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="11" t="s">
@@ -851,8 +850,8 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="2:9" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="16" t="s">
+    <row r="9" spans="2:9" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="11" t="s">

</xml_diff>